<commit_message>
Add interview and field observation templates for sports associations
</commit_message>
<xml_diff>
--- a/docs/fattibilita/template_gantt excell.xlsx
+++ b/docs/fattibilita/template_gantt excell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Desktop\scuola\5 INFO\GPOI\progetto-GPOI-5INFB-Guerini-Bertasa-Mutti-Zecchini\docs\fattibilita\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F253A4-AAE9-4A29-AAD1-A585CA93D6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11238867-E25A-4E58-B6B2-3A8AD68D0078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{9327F8D6-4F37-4E25-8083-20A17765DC2F}"/>
   </bookViews>
@@ -175,7 +175,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-410]"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +241,14 @@
     </font>
     <font>
       <sz val="25"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -482,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -638,6 +646,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -658,6 +669,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,7 +1055,7 @@
   <dimension ref="C2:AV39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1059,78 +1073,78 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:48" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="65"/>
+      <c r="D2" s="66"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="3:48" x14ac:dyDescent="0.45">
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="61"/>
+      <c r="D3" s="62"/>
       <c r="H3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="62" t="str">
+      <c r="I3" s="63" t="str">
         <f>TEXT(I5,"MMM")</f>
         <v>Oct</v>
       </c>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="62" t="str">
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="63" t="str">
         <f>TEXT(M5,"MMM")</f>
         <v>Nov</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="62" t="str">
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="63" t="str">
         <f>TEXT(Q5,"MMM")</f>
         <v>Dec</v>
       </c>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
       <c r="U3" s="7"/>
-      <c r="V3" s="62" t="str">
+      <c r="V3" s="63" t="str">
         <f>TEXT(V5,"MMM")</f>
         <v>Jan</v>
       </c>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="62" t="str">
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="65"/>
+      <c r="Z3" s="63" t="str">
         <f>TEXT(Z5,"MMM")</f>
         <v>Feb</v>
       </c>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="62" t="str">
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="63" t="str">
         <f>TEXT(AD5,"MMM")</f>
         <v>Mar</v>
       </c>
-      <c r="AE3" s="63"/>
-      <c r="AF3" s="63"/>
-      <c r="AG3" s="63"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
       <c r="AH3" s="7"/>
-      <c r="AI3" s="62" t="str">
+      <c r="AI3" s="63" t="str">
         <f>TEXT(AI5,"MMM")</f>
         <v>Apr</v>
       </c>
-      <c r="AJ3" s="63"/>
-      <c r="AK3" s="63"/>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="62" t="str">
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="64"/>
+      <c r="AL3" s="65"/>
+      <c r="AM3" s="63" t="str">
         <f>TEXT(AM5,"MMM")</f>
         <v>May</v>
       </c>
-      <c r="AN3" s="63"/>
-      <c r="AO3" s="63"/>
-      <c r="AP3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="65"/>
       <c r="AQ3" s="6" t="str">
         <f>TEXT(AQ5,"MMM")</f>
         <v>Jun</v>
@@ -1545,17 +1559,17 @@
         <v>20</v>
       </c>
       <c r="E9" s="27">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="F9" s="30">
         <v>45940</v>
       </c>
       <c r="G9" s="30">
-        <v>45941</v>
+        <v>45945</v>
       </c>
       <c r="H9" s="24"/>
       <c r="I9" s="25">
-        <f t="shared" ref="I8:I26" si="1">1*AND(I$5&gt;=task_start,I$5&lt;=task_start+(task_progress*(task_end-task_start+1))-1)</f>
+        <f t="shared" ref="I9:I26" si="1">1*AND(I$5&gt;=task_start,I$5&lt;=task_start+(task_progress*(task_end-task_start+1))-1)</f>
         <v>0</v>
       </c>
       <c r="J9" s="25"/>
@@ -1810,7 +1824,7 @@
         <v>45964</v>
       </c>
       <c r="G13" s="30">
-        <v>45964</v>
+        <v>45967</v>
       </c>
       <c r="H13" s="24"/>
       <c r="I13" s="25">
@@ -1877,8 +1891,8 @@
       <c r="F14" s="30">
         <v>45962</v>
       </c>
-      <c r="G14" s="30">
-        <v>46022</v>
+      <c r="G14" s="59">
+        <v>45962</v>
       </c>
       <c r="H14" s="24"/>
       <c r="I14" s="25">
@@ -1921,15 +1935,15 @@
       <c r="AQ14" s="23"/>
       <c r="AS14" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AT14" s="53">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU14" s="55">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="AV14" t="s">
         <v>35</v>
@@ -1949,7 +1963,7 @@
         <v>45962</v>
       </c>
       <c r="G15" s="30">
-        <v>46022</v>
+        <v>45962</v>
       </c>
       <c r="H15" s="24"/>
       <c r="I15" s="25">
@@ -1992,15 +2006,15 @@
       <c r="AQ15" s="23"/>
       <c r="AS15" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AT15" s="53">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU15" s="55">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="3:48" ht="21" customHeight="1" x14ac:dyDescent="0.45">
@@ -2017,7 +2031,7 @@
         <v>45962</v>
       </c>
       <c r="G16" s="30">
-        <v>46022</v>
+        <v>45962</v>
       </c>
       <c r="H16" s="24"/>
       <c r="I16" s="25">
@@ -2060,15 +2074,15 @@
       <c r="AQ16" s="23"/>
       <c r="AS16" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AT16" s="53">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU16" s="55">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:47" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2145,7 +2159,7 @@
         <v>45945</v>
       </c>
       <c r="G18" s="30">
-        <v>46022</v>
+        <v>45962</v>
       </c>
       <c r="H18" s="24"/>
       <c r="I18" s="25">
@@ -2188,15 +2202,15 @@
       <c r="AQ18" s="23"/>
       <c r="AS18" s="8">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="AT18" s="53">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="AU18" s="55">
         <f t="shared" si="3"/>
-        <v>495</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.45">
@@ -2213,7 +2227,7 @@
         <v>45962</v>
       </c>
       <c r="G19" s="30">
-        <v>46022</v>
+        <v>45962</v>
       </c>
       <c r="H19" s="24"/>
       <c r="I19" s="25">
@@ -2256,15 +2270,15 @@
       <c r="AQ19" s="23"/>
       <c r="AS19" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AT19" s="53">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU19" s="55">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.45">
@@ -2281,7 +2295,7 @@
         <v>45962</v>
       </c>
       <c r="G20" s="30">
-        <v>46022</v>
+        <v>45962</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="25">
@@ -2324,15 +2338,15 @@
       <c r="AQ20" s="23"/>
       <c r="AS20" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AT20" s="53">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU20" s="55">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.45">
@@ -2349,7 +2363,7 @@
         <v>45962</v>
       </c>
       <c r="G21" s="30">
-        <v>46022</v>
+        <v>45962</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="25">
@@ -2392,15 +2406,15 @@
       <c r="AQ21" s="23"/>
       <c r="AS21" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AT21" s="53">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU21" s="55">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="3:47" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2547,7 +2561,7 @@
         <v>45962</v>
       </c>
       <c r="G24" s="30">
-        <v>46022</v>
+        <v>45962</v>
       </c>
       <c r="H24" s="24"/>
       <c r="I24" s="25">
@@ -2590,15 +2604,15 @@
       <c r="AQ24" s="23"/>
       <c r="AS24" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AT24" s="53">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU24" s="55">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.45">
@@ -2615,7 +2629,7 @@
         <v>45962</v>
       </c>
       <c r="G25" s="30">
-        <v>46022</v>
+        <v>45962</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="25">
@@ -2658,15 +2672,15 @@
       <c r="AQ25" s="23"/>
       <c r="AS25" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AT25" s="53">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU25" s="55">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.45">
@@ -2683,7 +2697,7 @@
         <v>45962</v>
       </c>
       <c r="G26" s="30">
-        <v>46022</v>
+        <v>45962</v>
       </c>
       <c r="H26" s="24"/>
       <c r="I26" s="25">
@@ -2726,15 +2740,15 @@
       <c r="AQ26" s="23"/>
       <c r="AS26" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AT26" s="53">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AU26" s="55">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="3:47" x14ac:dyDescent="0.45">
@@ -2760,50 +2774,51 @@
       <c r="C30" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="59" t="s">
+      <c r="D30" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="61"/>
       <c r="AS30" s="51">
         <f>SUM(AS8:AS26)</f>
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="AT30" s="54">
         <f>SUM(AT8:AT26)</f>
-        <v>252</v>
+        <v>9</v>
       </c>
       <c r="AU30" s="56">
         <f>SUM(AU8:AU26)</f>
-        <v>3780</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C31" s="42"/>
-      <c r="D31" s="59" t="s">
+      <c r="D31" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="59"/>
-      <c r="F31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="61"/>
     </row>
     <row r="32" spans="3:47" x14ac:dyDescent="0.45">
       <c r="C32" s="42"/>
-      <c r="D32" s="59" t="s">
+      <c r="D32" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="59"/>
-      <c r="F32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="61"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
+      <c r="M32" s="67"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C33" s="42"/>
-      <c r="D33" s="59" t="s">
+      <c r="D33" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="59"/>
-      <c r="F33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="61"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -2906,12 +2921,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:AP8 I9:AP11 I9:I26 Y13:AD26 AG13:AL26 AO13:AP26 I13:V26">
+  <conditionalFormatting sqref="H8:AP8 I9:AP11 I9:I26 I13:V26 Y13:AD26 AG13:AL26 AO13:AP26">
     <cfRule type="expression" dxfId="2" priority="10">
       <formula>AND(H$5&gt;=$F8,H$5&lt;=$G8)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:AP8 I5:AQ7 AQ8:AQ26 I9:AP26">
+  <conditionalFormatting sqref="H8:AP8 I9:AP26 I5:AQ7 AQ8:AQ26">
     <cfRule type="expression" dxfId="1" priority="13">
       <formula>AND(H$5&lt;=TODAY(), (I$5-7)&lt;=TODAY(),I$5&gt;=TODAY())</formula>
     </cfRule>

</xml_diff>